<commit_message>
📊 Update SwaadSutra_Daily_2026-01-14.xlsx - 2026-01-14T17:08:05.513Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-14.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-14.xlsx
@@ -399,13 +399,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Order ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Flat No</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Items</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Total</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Payment</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Collection Date</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Collection Time</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Notes</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Cancel Reason</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Feedback</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>14</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-01-14 17:08</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Mrunal</v>
+      </c>
+      <c r="D2" t="str">
+        <v>KLV B 2108</v>
+      </c>
+      <c r="E2" t="str">
+        <v>9404665203</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Wheat Chapati x40</v>
+      </c>
+      <c r="G2">
+        <v>600</v>
+      </c>
+      <c r="H2" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I2" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J2" t="str">
+        <v>2026-01-15</v>
+      </c>
+      <c r="K2" t="str">
+        <v>00:30</v>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -445,10 +534,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -463,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -478,13 +567,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Item</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Quantity Ordered</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Revenue</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Wheat Chapati</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>